<commit_message>
Update Pathway analysis of combined met and pro only p-value less than 0.05.xlsx
</commit_message>
<xml_diff>
--- a/Pathway analysis/Second pathway analysis only using p-value/Pathway analysis of combined met and pro only p-value less than 0.05.xlsx
+++ b/Pathway analysis/Second pathway analysis only using p-value/Pathway analysis of combined met and pro only p-value less than 0.05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\Pathway analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\Pathway analysis\Second pathway analysis only using p-value\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{35727D75-6B41-47DB-A725-9C057587FCF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0953AED5-5543-4016-BF11-C29A19A46B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="9710" yWindow="540" windowWidth="9490" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pathway analysis of combined me" sheetId="1" r:id="rId1"/>
@@ -1819,7 +1819,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1956,7 +1956,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2136,6 +2136,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -2297,10 +2303,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2655,11 +2663,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G590"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2831,26 +2839,26 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>8</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>116</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>0.375</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>2.63</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>0.04</v>
       </c>
     </row>

</xml_diff>